<commit_message>
adding std of accuracies for result analysis
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F857F39F-E65F-4B47-939F-7E00B2698C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EFA0AC-121D-4B29-88DF-B7CDB32E4EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
     <sheet name="acc_mean" sheetId="1" r:id="rId2"/>
-    <sheet name="acc_median" sheetId="7" r:id="rId3"/>
-    <sheet name="nprot_best" sheetId="3" r:id="rId4"/>
-    <sheet name="nprot_mean" sheetId="8" r:id="rId5"/>
-    <sheet name="K_best" sheetId="9" r:id="rId6"/>
-    <sheet name="K_mean" sheetId="10" r:id="rId7"/>
-    <sheet name="hp_best" sheetId="12" r:id="rId8"/>
-    <sheet name="v1_v2_best" sheetId="13" r:id="rId9"/>
-    <sheet name="MCC" sheetId="14" r:id="rId10"/>
-    <sheet name="F1S" sheetId="15" r:id="rId11"/>
+    <sheet name="acc_std" sheetId="16" r:id="rId3"/>
+    <sheet name="acc_median" sheetId="7" r:id="rId4"/>
+    <sheet name="nprot_best" sheetId="3" r:id="rId5"/>
+    <sheet name="nprot_mean" sheetId="8" r:id="rId6"/>
+    <sheet name="K_best" sheetId="9" r:id="rId7"/>
+    <sheet name="K_mean" sheetId="10" r:id="rId8"/>
+    <sheet name="hp_best" sheetId="12" r:id="rId9"/>
+    <sheet name="v1_v2_best" sheetId="13" r:id="rId10"/>
+    <sheet name="MCC" sheetId="14" r:id="rId11"/>
+    <sheet name="F1S" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="37">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -154,6 +155,9 @@
   </si>
   <si>
     <t>Sparsification Method</t>
+  </si>
+  <si>
+    <t>Cervical Cancer DataSet 02 - hold 02 - Accuracy (std)</t>
   </si>
 </sst>
 </file>
@@ -646,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -933,6 +937,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -960,7 +967,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1246,7 +1286,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,19 +1304,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2170,6 +2210,1230 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
+  <dimension ref="A1:S53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="103"/>
+      <c r="F3" s="102" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="103"/>
+      <c r="H3" s="102" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="103"/>
+      <c r="J3" s="102" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="103"/>
+      <c r="L3" s="102" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="103"/>
+      <c r="N3" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="103"/>
+      <c r="P3" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="104"/>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="I5" s="27"/>
+      <c r="J5" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="K5" s="27"/>
+      <c r="L5" s="54">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="12">
+        <v>-1.953125E-3</v>
+      </c>
+      <c r="O5" s="27"/>
+      <c r="P5" s="28">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="28">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="S5" s="27"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29">
+        <v>1</v>
+      </c>
+      <c r="K6" s="29"/>
+      <c r="L6" s="13">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="M6" s="29"/>
+      <c r="N6" s="31">
+        <v>-1.5625E-2</v>
+      </c>
+      <c r="O6" s="29"/>
+      <c r="P6" s="31">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="S6" s="29"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="29">
+        <v>16</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29">
+        <v>8</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="J7" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="M7" s="29"/>
+      <c r="N7" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="O7" s="29"/>
+      <c r="P7" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="29"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="29">
+        <v>4</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29">
+        <v>1</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="M8" s="29"/>
+      <c r="N8" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="O8" s="29"/>
+      <c r="P8" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="S8" s="29"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="K9" s="29"/>
+      <c r="L9" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="M9" s="29"/>
+      <c r="N9" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="29"/>
+      <c r="P9" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="S9" s="29"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30">
+        <v>0.999</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="K10" s="29"/>
+      <c r="L10" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="M10" s="29"/>
+      <c r="N10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="O10" s="29"/>
+      <c r="P10" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29">
+        <v>0.999</v>
+      </c>
+      <c r="S10" s="29"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="M11" s="29"/>
+      <c r="N11" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="O11" s="29"/>
+      <c r="P11" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29">
+        <v>0.999</v>
+      </c>
+      <c r="S11" s="29"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="29"/>
+      <c r="L12" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="M12" s="29"/>
+      <c r="N12" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="O12" s="29"/>
+      <c r="P12" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="S12" s="29"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29">
+        <v>32</v>
+      </c>
+      <c r="E13" s="29">
+        <v>64.0009765625</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="H13" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="I13" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="J13" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K13" s="29">
+        <v>8.0009765625</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="M13" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="N13" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="O13" s="29">
+        <v>256.0009765625</v>
+      </c>
+      <c r="P13" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>2.0009765625</v>
+      </c>
+      <c r="R13" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="S13" s="29">
+        <v>1.0009765625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="29">
+        <v>16</v>
+      </c>
+      <c r="E14" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="G14" s="29">
+        <v>512.0009765625</v>
+      </c>
+      <c r="H14" s="31">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="I14" s="31">
+        <v>6.34765625E-2</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="K14" s="29">
+        <v>1.0009765625</v>
+      </c>
+      <c r="L14" s="29">
+        <v>1</v>
+      </c>
+      <c r="M14" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="O14" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="P14" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="R14" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="S14" s="29">
+        <v>4.0009765625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
+        <v>128</v>
+      </c>
+      <c r="E15" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="F15" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G15" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="H15" s="29">
+        <v>512</v>
+      </c>
+      <c r="I15" s="19">
+        <v>6.34765625E-2</v>
+      </c>
+      <c r="J15" s="31">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="K15" s="13">
+        <v>3.22265625E-2</v>
+      </c>
+      <c r="L15" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="M15" s="31">
+        <v>3.22265625E-2</v>
+      </c>
+      <c r="N15" s="29">
+        <v>256</v>
+      </c>
+      <c r="O15" s="13">
+        <v>8.7890625E-3</v>
+      </c>
+      <c r="P15" s="29">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="R15" s="29">
+        <v>16</v>
+      </c>
+      <c r="S15" s="13">
+        <v>6.34765625E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0.5009765625</v>
+      </c>
+      <c r="F16" s="29">
+        <v>32</v>
+      </c>
+      <c r="G16" s="29">
+        <v>512.0009765625</v>
+      </c>
+      <c r="H16" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="I16" s="29">
+        <v>256.0009765625</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="29">
+        <v>1.0009765625</v>
+      </c>
+      <c r="L16" s="29">
+        <v>1024</v>
+      </c>
+      <c r="M16" s="31">
+        <v>1.66015625E-2</v>
+      </c>
+      <c r="N16" s="29">
+        <v>1</v>
+      </c>
+      <c r="O16" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="P16" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="R16" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="S16" s="29">
+        <v>512.0009765625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29">
+        <v>2</v>
+      </c>
+      <c r="E17" s="29">
+        <v>8.0009765625</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="29">
+        <v>1.0009765625</v>
+      </c>
+      <c r="H17" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="29">
+        <v>64.0009765625</v>
+      </c>
+      <c r="J17" s="29">
+        <v>32</v>
+      </c>
+      <c r="K17" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="L17" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M17" s="19">
+        <v>0.1259765625</v>
+      </c>
+      <c r="N17" s="30">
+        <v>-0.25</v>
+      </c>
+      <c r="O17" s="29">
+        <v>64.0009765625</v>
+      </c>
+      <c r="P17" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="R17" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S17" s="29">
+        <v>256.0009765625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="29">
+        <v>1</v>
+      </c>
+      <c r="E18" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="F18" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="29">
+        <v>1.0009765625</v>
+      </c>
+      <c r="H18" s="29">
+        <v>4</v>
+      </c>
+      <c r="I18" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="J18" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="K18" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="L18" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="M18" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="N18" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="O18" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="P18" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>64.0009765625</v>
+      </c>
+      <c r="R18" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="S18" s="29">
+        <v>8.0009765625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="29">
+        <v>2</v>
+      </c>
+      <c r="E19" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="F19" s="30">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G19" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="H19" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="I19" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="J19" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="L19" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="M19" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="N19" s="29">
+        <v>-32</v>
+      </c>
+      <c r="O19" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="P19" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="Q19" s="29">
+        <v>0.5009765625</v>
+      </c>
+      <c r="R19" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S19" s="29">
+        <v>4.0009765625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="F20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="H20" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="I20" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="J20" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K20" s="30">
+        <v>0.5009765625</v>
+      </c>
+      <c r="L20" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="M20" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="N20" s="31">
+        <v>-3.125E-2</v>
+      </c>
+      <c r="O20" s="31">
+        <v>-6.8359375E-3</v>
+      </c>
+      <c r="P20" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q20" s="13">
+        <v>0.5009765625</v>
+      </c>
+      <c r="R20" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="S20" s="29">
+        <v>8.0009765625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+    </row>
+    <row r="49" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+    </row>
+    <row r="50" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+    </row>
+    <row r="51" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+    </row>
+    <row r="52" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+    </row>
+    <row r="53" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8065C56F-AEED-4D36-9CB5-AF6203A45422}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2185,19 +3449,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2772,7 +4036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF1E589-1659-439B-B1DA-4F9E028A9755}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2788,19 +4052,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3380,7 +4644,7 @@
   <dimension ref="A1:W53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3400,48 +4664,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99"/>
-      <c r="M3" s="97" t="s">
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="100"/>
+      <c r="M3" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="98"/>
-      <c r="W3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="100"/>
     </row>
     <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -4654,32 +5918,32 @@
       <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="97" t="s">
+      <c r="A22" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="98"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="98"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="99"/>
-      <c r="M22" s="97" t="s">
+      <c r="B22" s="99"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="100"/>
+      <c r="M22" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="N22" s="98"/>
-      <c r="O22" s="98"/>
-      <c r="P22" s="98"/>
-      <c r="Q22" s="98"/>
-      <c r="R22" s="98"/>
-      <c r="S22" s="98"/>
-      <c r="T22" s="98"/>
-      <c r="U22" s="98"/>
-      <c r="V22" s="98"/>
-      <c r="W22" s="99"/>
+      <c r="N22" s="99"/>
+      <c r="O22" s="99"/>
+      <c r="P22" s="99"/>
+      <c r="Q22" s="99"/>
+      <c r="R22" s="99"/>
+      <c r="S22" s="99"/>
+      <c r="T22" s="99"/>
+      <c r="U22" s="99"/>
+      <c r="V22" s="99"/>
+      <c r="W22" s="100"/>
     </row>
     <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
@@ -4715,7 +5979,7 @@
       <c r="K23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M23" s="105" t="s">
+      <c r="M23" s="96" t="s">
         <v>35</v>
       </c>
       <c r="N23" s="3" t="s">
@@ -6162,6 +7426,627 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5CD397-A860-45CD-AB1F-382D2CA5649F}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="98" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="100"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="106">
+        <v>7.0292878838302403E-2</v>
+      </c>
+      <c r="E5" s="107">
+        <v>6.3885385472767606E-2</v>
+      </c>
+      <c r="F5" s="107">
+        <v>4.4733445495905501E-2</v>
+      </c>
+      <c r="G5" s="107">
+        <v>8.6709886175555195E-2</v>
+      </c>
+      <c r="H5" s="107">
+        <v>7.9100517117031394E-2</v>
+      </c>
+      <c r="I5" s="107">
+        <v>0.122139770667702</v>
+      </c>
+      <c r="J5" s="107">
+        <v>7.6110976062704797E-2</v>
+      </c>
+      <c r="K5" s="108">
+        <v>8.8161696538346906E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="109">
+        <v>4.2788495511944802E-2</v>
+      </c>
+      <c r="E6" s="110">
+        <v>3.5462695040305602E-2</v>
+      </c>
+      <c r="F6" s="110">
+        <v>3.25693504546265E-2</v>
+      </c>
+      <c r="G6" s="110">
+        <v>3.5993780314161797E-2</v>
+      </c>
+      <c r="H6" s="110">
+        <v>3.3786099594715603E-2</v>
+      </c>
+      <c r="I6" s="110">
+        <v>1.23058257323665E-2</v>
+      </c>
+      <c r="J6" s="110">
+        <v>6.4294961094221698E-2</v>
+      </c>
+      <c r="K6" s="111">
+        <v>7.0608786565813597E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="109">
+        <v>4.8340046085368002E-2</v>
+      </c>
+      <c r="E7" s="110">
+        <v>3.8968058326434803E-2</v>
+      </c>
+      <c r="F7" s="110">
+        <v>5.2556559774448799E-2</v>
+      </c>
+      <c r="G7" s="110">
+        <v>6.9763503820971004E-2</v>
+      </c>
+      <c r="H7" s="110">
+        <v>5.7371272929003903E-2</v>
+      </c>
+      <c r="I7" s="110">
+        <v>3.1979376676930502E-2</v>
+      </c>
+      <c r="J7" s="110">
+        <v>2.93756383587572E-2</v>
+      </c>
+      <c r="K7" s="111">
+        <v>5.2076349704757899E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="112">
+        <v>3.4158780366309899E-2</v>
+      </c>
+      <c r="E8" s="113">
+        <v>3.00808053255281E-2</v>
+      </c>
+      <c r="F8" s="113">
+        <v>3.1896356348196403E-2</v>
+      </c>
+      <c r="G8" s="113">
+        <v>5.9329490470541799E-2</v>
+      </c>
+      <c r="H8" s="113">
+        <v>4.75450276627171E-2</v>
+      </c>
+      <c r="I8" s="113">
+        <v>2.1309649902165301E-2</v>
+      </c>
+      <c r="J8" s="113">
+        <v>3.01550865042849E-2</v>
+      </c>
+      <c r="K8" s="114">
+        <v>3.5945404961161803E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="115">
+        <v>2.72479531927605E-2</v>
+      </c>
+      <c r="E9" s="116">
+        <v>5.7362895599682898E-2</v>
+      </c>
+      <c r="F9" s="116">
+        <v>2.2677233246521399E-2</v>
+      </c>
+      <c r="G9" s="116">
+        <v>4.4183267367529998E-2</v>
+      </c>
+      <c r="H9" s="116">
+        <v>8.3625223719074507E-2</v>
+      </c>
+      <c r="I9" s="116">
+        <v>0.38618348621941501</v>
+      </c>
+      <c r="J9" s="116">
+        <v>3.7690011061215702E-2</v>
+      </c>
+      <c r="K9" s="117">
+        <v>4.78358745331341E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="109">
+        <v>3.5722034569767303E-2</v>
+      </c>
+      <c r="E10" s="110">
+        <v>8.7643630574284995E-2</v>
+      </c>
+      <c r="F10" s="110">
+        <v>4.59281460693012E-2</v>
+      </c>
+      <c r="G10" s="110">
+        <v>4.7123856398196301E-2</v>
+      </c>
+      <c r="H10" s="110">
+        <v>4.33058935567468E-2</v>
+      </c>
+      <c r="I10" s="110">
+        <v>0.39414687013612798</v>
+      </c>
+      <c r="J10" s="110">
+        <v>5.73756055504204E-2</v>
+      </c>
+      <c r="K10" s="111">
+        <v>7.7418121207890503E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="109">
+        <v>4.8733371962992801E-2</v>
+      </c>
+      <c r="E11" s="110">
+        <v>8.3294222931895603E-2</v>
+      </c>
+      <c r="F11" s="110">
+        <v>4.7210988843555603E-2</v>
+      </c>
+      <c r="G11" s="110">
+        <v>3.5207564424687803E-2</v>
+      </c>
+      <c r="H11" s="110">
+        <v>4.0947578948443197E-2</v>
+      </c>
+      <c r="I11" s="110">
+        <v>0.15970409909161201</v>
+      </c>
+      <c r="J11" s="110">
+        <v>5.9824611494191701E-2</v>
+      </c>
+      <c r="K11" s="111">
+        <v>5.7350182832165503E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="112">
+        <v>4.5792638401643403E-2</v>
+      </c>
+      <c r="E12" s="113">
+        <v>3.6144020191137799E-2</v>
+      </c>
+      <c r="F12" s="113">
+        <v>2.3416416937499001E-2</v>
+      </c>
+      <c r="G12" s="113">
+        <v>4.4485664319080603E-2</v>
+      </c>
+      <c r="H12" s="113">
+        <v>6.2823133520800198E-2</v>
+      </c>
+      <c r="I12" s="113">
+        <v>0.22570171277814199</v>
+      </c>
+      <c r="J12" s="113">
+        <v>3.51043321099287E-2</v>
+      </c>
+      <c r="K12" s="114">
+        <v>7.2621285334136004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="115">
+        <v>2.9190583322558899E-2</v>
+      </c>
+      <c r="E13" s="116">
+        <v>5.5541683205126001E-2</v>
+      </c>
+      <c r="F13" s="116">
+        <v>3.4334917584273698E-2</v>
+      </c>
+      <c r="G13" s="116">
+        <v>5.6529446942684101E-2</v>
+      </c>
+      <c r="H13" s="116">
+        <v>4.3852341385341498E-2</v>
+      </c>
+      <c r="I13" s="116">
+        <v>3.5170360307989597E-2</v>
+      </c>
+      <c r="J13" s="116">
+        <v>5.3986296417612399E-2</v>
+      </c>
+      <c r="K13" s="117">
+        <v>3.0753654409090999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="109">
+        <v>3.4619468621401597E-2</v>
+      </c>
+      <c r="E14" s="110">
+        <v>3.75137237942312E-2</v>
+      </c>
+      <c r="F14" s="110">
+        <v>2.9199097751376302E-2</v>
+      </c>
+      <c r="G14" s="110">
+        <v>4.0217451082638501E-2</v>
+      </c>
+      <c r="H14" s="110">
+        <v>4.47427059668997E-2</v>
+      </c>
+      <c r="I14" s="110">
+        <v>5.5239210176038202E-2</v>
+      </c>
+      <c r="J14" s="110">
+        <v>7.7189385374219099E-2</v>
+      </c>
+      <c r="K14" s="111">
+        <v>4.5046497788515001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="109">
+        <v>0.24706066856558201</v>
+      </c>
+      <c r="E15" s="110">
+        <v>0.33740040389728299</v>
+      </c>
+      <c r="F15" s="110">
+        <v>0.27435027637128701</v>
+      </c>
+      <c r="G15" s="110">
+        <v>0.36488995555502002</v>
+      </c>
+      <c r="H15" s="110">
+        <v>0.27745194034564402</v>
+      </c>
+      <c r="I15" s="110">
+        <v>0.16087114350569401</v>
+      </c>
+      <c r="J15" s="110">
+        <v>0.26645694645615797</v>
+      </c>
+      <c r="K15" s="111">
+        <v>0.39284887009292502</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="112">
+        <v>0.26533929071968798</v>
+      </c>
+      <c r="E16" s="113">
+        <v>0.365503463516896</v>
+      </c>
+      <c r="F16" s="113">
+        <v>0.13317394967899401</v>
+      </c>
+      <c r="G16" s="113">
+        <v>0.33252053833431999</v>
+      </c>
+      <c r="H16" s="113">
+        <v>0.21896674606156</v>
+      </c>
+      <c r="I16" s="113">
+        <v>0.185980773261017</v>
+      </c>
+      <c r="J16" s="113">
+        <v>0.25420245104004202</v>
+      </c>
+      <c r="K16" s="114">
+        <v>0.38532622989967402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="115">
+        <v>0.21162974698353201</v>
+      </c>
+      <c r="E17" s="116">
+        <v>2.34142937376756E-2</v>
+      </c>
+      <c r="F17" s="116">
+        <v>2.8533150420674398E-2</v>
+      </c>
+      <c r="G17" s="116">
+        <v>6.2531236300992402E-2</v>
+      </c>
+      <c r="H17" s="116">
+        <v>4.8321187430193202E-2</v>
+      </c>
+      <c r="I17" s="116">
+        <v>4.8215098943489E-2</v>
+      </c>
+      <c r="J17" s="116">
+        <v>6.08128428659322E-2</v>
+      </c>
+      <c r="K17" s="117">
+        <v>4.8039144037443499E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="109">
+        <v>0.19599022212167</v>
+      </c>
+      <c r="E18" s="110">
+        <v>7.1850458677384904E-2</v>
+      </c>
+      <c r="F18" s="110">
+        <v>3.8092810837237499E-2</v>
+      </c>
+      <c r="G18" s="110">
+        <v>2.9919507057879401E-2</v>
+      </c>
+      <c r="H18" s="110">
+        <v>5.0702605851674798E-2</v>
+      </c>
+      <c r="I18" s="110">
+        <v>6.8041442632727003E-2</v>
+      </c>
+      <c r="J18" s="110">
+        <v>6.1245946663548802E-2</v>
+      </c>
+      <c r="K18" s="111">
+        <v>4.8590340696011702E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="109">
+        <v>4.3195544271502198E-2</v>
+      </c>
+      <c r="E19" s="110">
+        <v>7.0609960052089499E-2</v>
+      </c>
+      <c r="F19" s="110">
+        <v>2.3439052435232199E-2</v>
+      </c>
+      <c r="G19" s="110">
+        <v>8.3216992476117302E-2</v>
+      </c>
+      <c r="H19" s="110">
+        <v>5.8001838540679002E-2</v>
+      </c>
+      <c r="I19" s="110">
+        <v>4.0420903990747499E-2</v>
+      </c>
+      <c r="J19" s="110">
+        <v>6.8142929336175301E-2</v>
+      </c>
+      <c r="K19" s="111">
+        <v>6.0469333439408898E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="112">
+        <v>4.6457664943769801E-2</v>
+      </c>
+      <c r="E20" s="113">
+        <v>4.7468284695804601E-2</v>
+      </c>
+      <c r="F20" s="113">
+        <v>6.9040477160007593E-2</v>
+      </c>
+      <c r="G20" s="113">
+        <v>6.1995729571322503E-2</v>
+      </c>
+      <c r="H20" s="113">
+        <v>7.6460288189190595E-2</v>
+      </c>
+      <c r="I20" s="113">
+        <v>6.2102826744178503E-2</v>
+      </c>
+      <c r="J20" s="113">
+        <v>2.4606937685458002E-2</v>
+      </c>
+      <c r="K20" s="114">
+        <v>5.3190927115455901E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E17B74-8A06-473F-B1B4-0C752BEBC712}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -6184,19 +8069,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6931,7 +8816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D980D9F8-6B96-4F95-8395-B1BF7462FEB8}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -6955,19 +8840,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7702,7 +9587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D696DEA4-1C6D-43BD-8BC6-2C617DFECF13}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -7725,19 +9610,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8472,7 +10357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40056-F547-48DD-9331-37B657810592}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -8495,19 +10380,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9242,7 +11127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5843C1-20CB-4050-94D7-D7DDEA36873C}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -9265,19 +11150,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10012,7 +11897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C6E2BB-CD7E-4FA9-A81B-F3147CB217E2}">
   <dimension ref="A1:P53"/>
   <sheetViews>
@@ -10041,24 +11926,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10068,29 +11953,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="100" t="s">
+      <c r="F3" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="101" t="s">
+      <c r="K3" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="102"/>
-      <c r="M3" s="101" t="s">
+      <c r="L3" s="103"/>
+      <c r="M3" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="102"/>
-      <c r="O3" s="101" t="s">
+      <c r="N3" s="103"/>
+      <c r="O3" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="103"/>
+      <c r="P3" s="104"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -11149,1228 +13034,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
-  <dimension ref="A1:S53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="102"/>
-      <c r="F3" s="101" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="102"/>
-      <c r="H3" s="101" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="102"/>
-      <c r="J3" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="102"/>
-      <c r="L3" s="101" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="102"/>
-      <c r="N3" s="101" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="102"/>
-      <c r="P3" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="101" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="103"/>
-    </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="27">
-        <v>1</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="12">
-        <v>0.125</v>
-      </c>
-      <c r="K5" s="27"/>
-      <c r="L5" s="54">
-        <v>0.5</v>
-      </c>
-      <c r="M5" s="27"/>
-      <c r="N5" s="12">
-        <v>-1.953125E-3</v>
-      </c>
-      <c r="O5" s="27"/>
-      <c r="P5" s="28">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="28">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="S5" s="27"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29">
-        <v>1</v>
-      </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="13">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="M6" s="29"/>
-      <c r="N6" s="31">
-        <v>-1.5625E-2</v>
-      </c>
-      <c r="O6" s="29"/>
-      <c r="P6" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="31">
-        <v>0.125</v>
-      </c>
-      <c r="S6" s="29"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="29">
-        <v>16</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29">
-        <v>8</v>
-      </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="S7" s="29"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="29">
-        <v>4</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29">
-        <v>1</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="M8" s="29"/>
-      <c r="N8" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="S8" s="29"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="O9" s="29"/>
-      <c r="P9" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="S9" s="29"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30">
-        <v>0.999</v>
-      </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30">
-        <v>0.6</v>
-      </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29">
-        <v>0.999</v>
-      </c>
-      <c r="S10" s="29"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30">
-        <v>0.01</v>
-      </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="30">
-        <v>1E-4</v>
-      </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="19">
-        <v>0.7</v>
-      </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29">
-        <v>0.999</v>
-      </c>
-      <c r="S11" s="29"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="M12" s="29"/>
-      <c r="N12" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="30">
-        <v>0.4</v>
-      </c>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="S12" s="29"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="29">
-        <v>32</v>
-      </c>
-      <c r="E13" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="F13" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="H13" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="I13" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="J13" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K13" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="L13" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="M13" s="30">
-        <v>0.2509765625</v>
-      </c>
-      <c r="N13" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="O13" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="P13" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q13" s="19">
-        <v>2.0009765625</v>
-      </c>
-      <c r="R13" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="S13" s="29">
-        <v>1.0009765625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="29">
-        <v>16</v>
-      </c>
-      <c r="E14" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="F14" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="G14" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="H14" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="I14" s="31">
-        <v>6.34765625E-2</v>
-      </c>
-      <c r="J14" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="K14" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="L14" s="29">
-        <v>1</v>
-      </c>
-      <c r="M14" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="N14" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="O14" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="P14" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="Q14" s="30">
-        <v>0.2509765625</v>
-      </c>
-      <c r="R14" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="S14" s="29">
-        <v>4.0009765625</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="29">
-        <v>128</v>
-      </c>
-      <c r="E15" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="F15" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="G15" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="H15" s="29">
-        <v>512</v>
-      </c>
-      <c r="I15" s="19">
-        <v>6.34765625E-2</v>
-      </c>
-      <c r="J15" s="31">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="K15" s="13">
-        <v>3.22265625E-2</v>
-      </c>
-      <c r="L15" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M15" s="31">
-        <v>3.22265625E-2</v>
-      </c>
-      <c r="N15" s="29">
-        <v>256</v>
-      </c>
-      <c r="O15" s="13">
-        <v>8.7890625E-3</v>
-      </c>
-      <c r="P15" s="29">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="R15" s="29">
-        <v>16</v>
-      </c>
-      <c r="S15" s="13">
-        <v>6.34765625E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="E16" s="29">
-        <v>0.5009765625</v>
-      </c>
-      <c r="F16" s="29">
-        <v>32</v>
-      </c>
-      <c r="G16" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="H16" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="I16" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="J16" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="K16" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="L16" s="29">
-        <v>1024</v>
-      </c>
-      <c r="M16" s="31">
-        <v>1.66015625E-2</v>
-      </c>
-      <c r="N16" s="29">
-        <v>1</v>
-      </c>
-      <c r="O16" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="P16" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="Q16" s="30">
-        <v>0.2509765625</v>
-      </c>
-      <c r="R16" s="31">
-        <v>0.125</v>
-      </c>
-      <c r="S16" s="29">
-        <v>512.0009765625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="29">
-        <v>2</v>
-      </c>
-      <c r="E17" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="F17" s="31">
-        <v>0.25</v>
-      </c>
-      <c r="G17" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="H17" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="J17" s="29">
-        <v>32</v>
-      </c>
-      <c r="K17" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="L17" s="13">
-        <v>6.25E-2</v>
-      </c>
-      <c r="M17" s="19">
-        <v>0.1259765625</v>
-      </c>
-      <c r="N17" s="30">
-        <v>-0.25</v>
-      </c>
-      <c r="O17" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="P17" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q17" s="30">
-        <v>0.2509765625</v>
-      </c>
-      <c r="R17" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S17" s="29">
-        <v>256.0009765625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="29">
-        <v>1</v>
-      </c>
-      <c r="E18" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="F18" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="H18" s="29">
-        <v>4</v>
-      </c>
-      <c r="I18" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="J18" s="31">
-        <v>0.125</v>
-      </c>
-      <c r="K18" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="L18" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="M18" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="N18" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="O18" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="P18" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="Q18" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="R18" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="S18" s="29">
-        <v>8.0009765625</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="29">
-        <v>2</v>
-      </c>
-      <c r="E19" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="F19" s="30">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G19" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="H19" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="I19" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="J19" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="L19" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="M19" s="30">
-        <v>0.2509765625</v>
-      </c>
-      <c r="N19" s="29">
-        <v>-32</v>
-      </c>
-      <c r="O19" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="P19" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q19" s="29">
-        <v>0.5009765625</v>
-      </c>
-      <c r="R19" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S19" s="29">
-        <v>4.0009765625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="F20" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="H20" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="I20" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="J20" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="K20" s="30">
-        <v>0.5009765625</v>
-      </c>
-      <c r="L20" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="M20" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="N20" s="31">
-        <v>-3.125E-2</v>
-      </c>
-      <c r="O20" s="31">
-        <v>-6.8359375E-3</v>
-      </c>
-      <c r="P20" s="13">
-        <v>6.25E-2</v>
-      </c>
-      <c r="Q20" s="13">
-        <v>0.5009765625</v>
-      </c>
-      <c r="R20" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="S20" s="29">
-        <v>8.0009765625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-    </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-    </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-    </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-    </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-    </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-    </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-    </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-    </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-    </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-    </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-    </row>
-    <row r="47" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-    </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-    </row>
-    <row r="49" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="10"/>
-      <c r="R49" s="10"/>
-    </row>
-    <row r="50" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-    </row>
-    <row r="51" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="10"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
-    </row>
-    <row r="52" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="10"/>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
-      <c r="Q52" s="10"/>
-      <c r="R52" s="10"/>
-    </row>
-    <row r="53" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
-      <c r="Q53" s="10"/>
-      <c r="R53" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
started analysis of spark and datasets, with just 8 lines of tables
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EFA0AC-121D-4B29-88DF-B7CDB32E4EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAB9B43-1769-4FA6-8347-681744353993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_best" sheetId="11" r:id="rId1"/>
@@ -967,40 +967,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4643,8 +4643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7527,28 +7527,28 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="106">
+      <c r="D5" s="45">
         <v>7.0292878838302403E-2</v>
       </c>
-      <c r="E5" s="107">
+      <c r="E5" s="12">
         <v>6.3885385472767606E-2</v>
       </c>
-      <c r="F5" s="107">
+      <c r="F5" s="12">
         <v>4.4733445495905501E-2</v>
       </c>
-      <c r="G5" s="107">
+      <c r="G5" s="12">
         <v>8.6709886175555195E-2</v>
       </c>
-      <c r="H5" s="107">
+      <c r="H5" s="12">
         <v>7.9100517117031394E-2</v>
       </c>
-      <c r="I5" s="107">
+      <c r="I5" s="12">
         <v>0.122139770667702</v>
       </c>
-      <c r="J5" s="107">
+      <c r="J5" s="12">
         <v>7.6110976062704797E-2</v>
       </c>
-      <c r="K5" s="108">
+      <c r="K5" s="46">
         <v>8.8161696538346906E-2</v>
       </c>
     </row>
@@ -7558,28 +7558,28 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="109">
+      <c r="D6" s="47">
         <v>4.2788495511944802E-2</v>
       </c>
-      <c r="E6" s="110">
+      <c r="E6" s="13">
         <v>3.5462695040305602E-2</v>
       </c>
-      <c r="F6" s="110">
+      <c r="F6" s="13">
         <v>3.25693504546265E-2</v>
       </c>
-      <c r="G6" s="110">
+      <c r="G6" s="13">
         <v>3.5993780314161797E-2</v>
       </c>
-      <c r="H6" s="110">
+      <c r="H6" s="13">
         <v>3.3786099594715603E-2</v>
       </c>
-      <c r="I6" s="110">
+      <c r="I6" s="13">
         <v>1.23058257323665E-2</v>
       </c>
-      <c r="J6" s="110">
+      <c r="J6" s="13">
         <v>6.4294961094221698E-2</v>
       </c>
-      <c r="K6" s="111">
+      <c r="K6" s="15">
         <v>7.0608786565813597E-2</v>
       </c>
     </row>
@@ -7591,28 +7591,28 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="109">
+      <c r="D7" s="47">
         <v>4.8340046085368002E-2</v>
       </c>
-      <c r="E7" s="110">
+      <c r="E7" s="13">
         <v>3.8968058326434803E-2</v>
       </c>
-      <c r="F7" s="110">
+      <c r="F7" s="13">
         <v>5.2556559774448799E-2</v>
       </c>
-      <c r="G7" s="110">
+      <c r="G7" s="13">
         <v>6.9763503820971004E-2</v>
       </c>
-      <c r="H7" s="110">
+      <c r="H7" s="13">
         <v>5.7371272929003903E-2</v>
       </c>
-      <c r="I7" s="110">
+      <c r="I7" s="13">
         <v>3.1979376676930502E-2</v>
       </c>
-      <c r="J7" s="110">
+      <c r="J7" s="13">
         <v>2.93756383587572E-2</v>
       </c>
-      <c r="K7" s="111">
+      <c r="K7" s="15">
         <v>5.2076349704757899E-2</v>
       </c>
     </row>
@@ -7622,28 +7622,28 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="112">
+      <c r="D8" s="48">
         <v>3.4158780366309899E-2</v>
       </c>
-      <c r="E8" s="113">
+      <c r="E8" s="14">
         <v>3.00808053255281E-2</v>
       </c>
-      <c r="F8" s="113">
+      <c r="F8" s="14">
         <v>3.1896356348196403E-2</v>
       </c>
-      <c r="G8" s="113">
+      <c r="G8" s="14">
         <v>5.9329490470541799E-2</v>
       </c>
-      <c r="H8" s="113">
+      <c r="H8" s="14">
         <v>4.75450276627171E-2</v>
       </c>
-      <c r="I8" s="113">
+      <c r="I8" s="14">
         <v>2.1309649902165301E-2</v>
       </c>
-      <c r="J8" s="113">
+      <c r="J8" s="14">
         <v>3.01550865042849E-2</v>
       </c>
-      <c r="K8" s="114">
+      <c r="K8" s="49">
         <v>3.5945404961161803E-2</v>
       </c>
     </row>
@@ -7657,28 +7657,28 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="115">
+      <c r="D9" s="50">
         <v>2.72479531927605E-2</v>
       </c>
-      <c r="E9" s="116">
+      <c r="E9" s="51">
         <v>5.7362895599682898E-2</v>
       </c>
-      <c r="F9" s="116">
+      <c r="F9" s="51">
         <v>2.2677233246521399E-2</v>
       </c>
-      <c r="G9" s="116">
+      <c r="G9" s="51">
         <v>4.4183267367529998E-2</v>
       </c>
-      <c r="H9" s="116">
+      <c r="H9" s="51">
         <v>8.3625223719074507E-2</v>
       </c>
-      <c r="I9" s="116">
+      <c r="I9" s="51">
         <v>0.38618348621941501</v>
       </c>
-      <c r="J9" s="116">
+      <c r="J9" s="51">
         <v>3.7690011061215702E-2</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="52">
         <v>4.78358745331341E-2</v>
       </c>
     </row>
@@ -7688,28 +7688,28 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="109">
+      <c r="D10" s="47">
         <v>3.5722034569767303E-2</v>
       </c>
-      <c r="E10" s="110">
+      <c r="E10" s="13">
         <v>8.7643630574284995E-2</v>
       </c>
-      <c r="F10" s="110">
+      <c r="F10" s="13">
         <v>4.59281460693012E-2</v>
       </c>
-      <c r="G10" s="110">
+      <c r="G10" s="13">
         <v>4.7123856398196301E-2</v>
       </c>
-      <c r="H10" s="110">
+      <c r="H10" s="13">
         <v>4.33058935567468E-2</v>
       </c>
-      <c r="I10" s="110">
+      <c r="I10" s="13">
         <v>0.39414687013612798</v>
       </c>
-      <c r="J10" s="110">
+      <c r="J10" s="13">
         <v>5.73756055504204E-2</v>
       </c>
-      <c r="K10" s="111">
+      <c r="K10" s="15">
         <v>7.7418121207890503E-2</v>
       </c>
     </row>
@@ -7721,28 +7721,28 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="109">
+      <c r="D11" s="47">
         <v>4.8733371962992801E-2</v>
       </c>
-      <c r="E11" s="110">
+      <c r="E11" s="13">
         <v>8.3294222931895603E-2</v>
       </c>
-      <c r="F11" s="110">
+      <c r="F11" s="13">
         <v>4.7210988843555603E-2</v>
       </c>
-      <c r="G11" s="110">
+      <c r="G11" s="13">
         <v>3.5207564424687803E-2</v>
       </c>
-      <c r="H11" s="110">
+      <c r="H11" s="13">
         <v>4.0947578948443197E-2</v>
       </c>
-      <c r="I11" s="110">
+      <c r="I11" s="13">
         <v>0.15970409909161201</v>
       </c>
-      <c r="J11" s="110">
+      <c r="J11" s="13">
         <v>5.9824611494191701E-2</v>
       </c>
-      <c r="K11" s="111">
+      <c r="K11" s="15">
         <v>5.7350182832165503E-2</v>
       </c>
     </row>
@@ -7752,28 +7752,28 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="112">
+      <c r="D12" s="48">
         <v>4.5792638401643403E-2</v>
       </c>
-      <c r="E12" s="113">
+      <c r="E12" s="14">
         <v>3.6144020191137799E-2</v>
       </c>
-      <c r="F12" s="113">
+      <c r="F12" s="14">
         <v>2.3416416937499001E-2</v>
       </c>
-      <c r="G12" s="113">
+      <c r="G12" s="14">
         <v>4.4485664319080603E-2</v>
       </c>
-      <c r="H12" s="113">
+      <c r="H12" s="14">
         <v>6.2823133520800198E-2</v>
       </c>
-      <c r="I12" s="113">
+      <c r="I12" s="14">
         <v>0.22570171277814199</v>
       </c>
-      <c r="J12" s="113">
+      <c r="J12" s="14">
         <v>3.51043321099287E-2</v>
       </c>
-      <c r="K12" s="114">
+      <c r="K12" s="49">
         <v>7.2621285334136004E-2</v>
       </c>
     </row>
@@ -7787,28 +7787,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="115">
+      <c r="D13" s="50">
         <v>2.9190583322558899E-2</v>
       </c>
-      <c r="E13" s="116">
+      <c r="E13" s="51">
         <v>5.5541683205126001E-2</v>
       </c>
-      <c r="F13" s="116">
+      <c r="F13" s="51">
         <v>3.4334917584273698E-2</v>
       </c>
-      <c r="G13" s="116">
+      <c r="G13" s="51">
         <v>5.6529446942684101E-2</v>
       </c>
-      <c r="H13" s="116">
+      <c r="H13" s="51">
         <v>4.3852341385341498E-2</v>
       </c>
-      <c r="I13" s="116">
+      <c r="I13" s="51">
         <v>3.5170360307989597E-2</v>
       </c>
-      <c r="J13" s="116">
+      <c r="J13" s="51">
         <v>5.3986296417612399E-2</v>
       </c>
-      <c r="K13" s="117">
+      <c r="K13" s="52">
         <v>3.0753654409090999E-2</v>
       </c>
     </row>
@@ -7818,28 +7818,28 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="109">
+      <c r="D14" s="47">
         <v>3.4619468621401597E-2</v>
       </c>
-      <c r="E14" s="110">
+      <c r="E14" s="13">
         <v>3.75137237942312E-2</v>
       </c>
-      <c r="F14" s="110">
+      <c r="F14" s="13">
         <v>2.9199097751376302E-2</v>
       </c>
-      <c r="G14" s="110">
+      <c r="G14" s="13">
         <v>4.0217451082638501E-2</v>
       </c>
-      <c r="H14" s="110">
+      <c r="H14" s="13">
         <v>4.47427059668997E-2</v>
       </c>
-      <c r="I14" s="110">
+      <c r="I14" s="13">
         <v>5.5239210176038202E-2</v>
       </c>
-      <c r="J14" s="110">
+      <c r="J14" s="13">
         <v>7.7189385374219099E-2</v>
       </c>
-      <c r="K14" s="111">
+      <c r="K14" s="15">
         <v>4.5046497788515001E-2</v>
       </c>
     </row>
@@ -7851,28 +7851,28 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="109">
+      <c r="D15" s="47">
         <v>0.24706066856558201</v>
       </c>
-      <c r="E15" s="110">
+      <c r="E15" s="13">
         <v>0.33740040389728299</v>
       </c>
-      <c r="F15" s="110">
+      <c r="F15" s="13">
         <v>0.27435027637128701</v>
       </c>
-      <c r="G15" s="110">
+      <c r="G15" s="13">
         <v>0.36488995555502002</v>
       </c>
-      <c r="H15" s="110">
+      <c r="H15" s="13">
         <v>0.27745194034564402</v>
       </c>
-      <c r="I15" s="110">
+      <c r="I15" s="13">
         <v>0.16087114350569401</v>
       </c>
-      <c r="J15" s="110">
+      <c r="J15" s="13">
         <v>0.26645694645615797</v>
       </c>
-      <c r="K15" s="111">
+      <c r="K15" s="15">
         <v>0.39284887009292502</v>
       </c>
     </row>
@@ -7882,28 +7882,28 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="112">
+      <c r="D16" s="48">
         <v>0.26533929071968798</v>
       </c>
-      <c r="E16" s="113">
+      <c r="E16" s="14">
         <v>0.365503463516896</v>
       </c>
-      <c r="F16" s="113">
+      <c r="F16" s="14">
         <v>0.13317394967899401</v>
       </c>
-      <c r="G16" s="113">
+      <c r="G16" s="14">
         <v>0.33252053833431999</v>
       </c>
-      <c r="H16" s="113">
+      <c r="H16" s="14">
         <v>0.21896674606156</v>
       </c>
-      <c r="I16" s="113">
+      <c r="I16" s="14">
         <v>0.185980773261017</v>
       </c>
-      <c r="J16" s="113">
+      <c r="J16" s="14">
         <v>0.25420245104004202</v>
       </c>
-      <c r="K16" s="114">
+      <c r="K16" s="49">
         <v>0.38532622989967402</v>
       </c>
     </row>
@@ -7917,28 +7917,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="115">
+      <c r="D17" s="50">
         <v>0.21162974698353201</v>
       </c>
-      <c r="E17" s="116">
+      <c r="E17" s="51">
         <v>2.34142937376756E-2</v>
       </c>
-      <c r="F17" s="116">
+      <c r="F17" s="51">
         <v>2.8533150420674398E-2</v>
       </c>
-      <c r="G17" s="116">
+      <c r="G17" s="51">
         <v>6.2531236300992402E-2</v>
       </c>
-      <c r="H17" s="116">
+      <c r="H17" s="51">
         <v>4.8321187430193202E-2</v>
       </c>
-      <c r="I17" s="116">
+      <c r="I17" s="51">
         <v>4.8215098943489E-2</v>
       </c>
-      <c r="J17" s="116">
+      <c r="J17" s="51">
         <v>6.08128428659322E-2</v>
       </c>
-      <c r="K17" s="117">
+      <c r="K17" s="52">
         <v>4.8039144037443499E-2</v>
       </c>
     </row>
@@ -7948,28 +7948,28 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="109">
+      <c r="D18" s="47">
         <v>0.19599022212167</v>
       </c>
-      <c r="E18" s="110">
+      <c r="E18" s="13">
         <v>7.1850458677384904E-2</v>
       </c>
-      <c r="F18" s="110">
+      <c r="F18" s="13">
         <v>3.8092810837237499E-2</v>
       </c>
-      <c r="G18" s="110">
+      <c r="G18" s="13">
         <v>2.9919507057879401E-2</v>
       </c>
-      <c r="H18" s="110">
+      <c r="H18" s="13">
         <v>5.0702605851674798E-2</v>
       </c>
-      <c r="I18" s="110">
+      <c r="I18" s="13">
         <v>6.8041442632727003E-2</v>
       </c>
-      <c r="J18" s="110">
+      <c r="J18" s="13">
         <v>6.1245946663548802E-2</v>
       </c>
-      <c r="K18" s="111">
+      <c r="K18" s="15">
         <v>4.8590340696011702E-2</v>
       </c>
     </row>
@@ -7981,28 +7981,28 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="109">
+      <c r="D19" s="47">
         <v>4.3195544271502198E-2</v>
       </c>
-      <c r="E19" s="110">
+      <c r="E19" s="13">
         <v>7.0609960052089499E-2</v>
       </c>
-      <c r="F19" s="110">
+      <c r="F19" s="13">
         <v>2.3439052435232199E-2</v>
       </c>
-      <c r="G19" s="110">
+      <c r="G19" s="13">
         <v>8.3216992476117302E-2</v>
       </c>
-      <c r="H19" s="110">
+      <c r="H19" s="13">
         <v>5.8001838540679002E-2</v>
       </c>
-      <c r="I19" s="110">
+      <c r="I19" s="13">
         <v>4.0420903990747499E-2</v>
       </c>
-      <c r="J19" s="110">
+      <c r="J19" s="13">
         <v>6.8142929336175301E-2</v>
       </c>
-      <c r="K19" s="111">
+      <c r="K19" s="15">
         <v>6.0469333439408898E-2</v>
       </c>
     </row>
@@ -8012,28 +8012,28 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="112">
+      <c r="D20" s="48">
         <v>4.6457664943769801E-2</v>
       </c>
-      <c r="E20" s="113">
+      <c r="E20" s="14">
         <v>4.7468284695804601E-2</v>
       </c>
-      <c r="F20" s="113">
+      <c r="F20" s="14">
         <v>6.9040477160007593E-2</v>
       </c>
-      <c r="G20" s="113">
+      <c r="G20" s="14">
         <v>6.1995729571322503E-2</v>
       </c>
-      <c r="H20" s="113">
+      <c r="H20" s="14">
         <v>7.6460288189190595E-2</v>
       </c>
-      <c r="I20" s="113">
+      <c r="I20" s="14">
         <v>6.2102826744178503E-2</v>
       </c>
-      <c r="J20" s="113">
+      <c r="J20" s="14">
         <v>2.4606937685458002E-2</v>
       </c>
-      <c r="K20" s="114">
+      <c r="K20" s="49">
         <v>5.3190927115455901E-2</v>
       </c>
     </row>
@@ -8820,8 +8820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D980D9F8-6B96-4F95-8395-B1BF7462FEB8}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8900,28 +8900,28 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="106">
         <v>16</v>
       </c>
-      <c r="E5" s="66">
+      <c r="E5" s="107">
         <v>19</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="107">
         <v>19</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="107">
         <v>35</v>
       </c>
-      <c r="H5" s="54">
+      <c r="H5" s="107">
         <v>46</v>
       </c>
-      <c r="I5" s="66">
+      <c r="I5" s="107">
         <v>6</v>
       </c>
-      <c r="J5" s="66">
+      <c r="J5" s="107">
         <v>7</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="108">
         <v>22</v>
       </c>
     </row>
@@ -8930,28 +8930,28 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="68">
+      <c r="D6" s="109">
         <v>24</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="110">
         <v>53</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="110">
         <v>39</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="110">
         <v>3</v>
       </c>
-      <c r="H6" s="69">
+      <c r="H6" s="110">
         <v>4</v>
       </c>
-      <c r="I6" s="69">
+      <c r="I6" s="110">
         <v>270</v>
       </c>
-      <c r="J6" s="69">
+      <c r="J6" s="110">
         <v>14</v>
       </c>
-      <c r="K6" s="70">
+      <c r="K6" s="111">
         <v>9</v>
       </c>
     </row>
@@ -8963,28 +8963,28 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="109">
         <v>11</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="110">
         <v>12</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="110">
         <v>17</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="110">
         <v>15</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="110">
         <v>6</v>
       </c>
-      <c r="I7" s="69">
+      <c r="I7" s="110">
         <v>19</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="110">
         <v>5</v>
       </c>
-      <c r="K7" s="70">
+      <c r="K7" s="111">
         <v>12</v>
       </c>
     </row>
@@ -8994,28 +8994,28 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="72">
+      <c r="D8" s="112">
         <v>20</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="113">
         <v>23</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="113">
         <v>19</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="113">
         <v>16</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="113">
         <v>13</v>
       </c>
-      <c r="I8" s="73">
+      <c r="I8" s="113">
         <v>109</v>
       </c>
-      <c r="J8" s="73">
+      <c r="J8" s="113">
         <v>16</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="114">
         <v>38</v>
       </c>
     </row>
@@ -9029,28 +9029,28 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="115">
         <v>46</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="116">
         <v>4</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="116">
         <v>13</v>
       </c>
-      <c r="G9" s="76">
+      <c r="G9" s="116">
         <v>18</v>
       </c>
-      <c r="H9" s="77">
+      <c r="H9" s="116">
         <v>8</v>
       </c>
-      <c r="I9" s="76">
-        <v>1</v>
-      </c>
-      <c r="J9" s="77">
+      <c r="I9" s="116">
+        <v>1</v>
+      </c>
+      <c r="J9" s="116">
         <v>3</v>
       </c>
-      <c r="K9" s="78">
+      <c r="K9" s="117">
         <v>10</v>
       </c>
     </row>
@@ -9059,28 +9059,28 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="71">
+      <c r="D10" s="109">
         <v>18</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="110">
         <v>9</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F10" s="110">
         <v>89</v>
       </c>
-      <c r="G10" s="69">
+      <c r="G10" s="110">
         <v>49</v>
       </c>
-      <c r="H10" s="69">
+      <c r="H10" s="110">
         <v>48</v>
       </c>
-      <c r="I10" s="19">
-        <v>1</v>
-      </c>
-      <c r="J10" s="19">
+      <c r="I10" s="110">
+        <v>1</v>
+      </c>
+      <c r="J10" s="110">
         <v>49</v>
       </c>
-      <c r="K10" s="70">
+      <c r="K10" s="111">
         <v>27</v>
       </c>
     </row>
@@ -9092,28 +9092,28 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="68">
+      <c r="D11" s="109">
         <v>3</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="110">
         <v>23</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="110">
         <v>7</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="110">
         <v>19</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="110">
         <v>9</v>
       </c>
-      <c r="I11" s="69">
-        <v>2</v>
-      </c>
-      <c r="J11" s="19">
+      <c r="I11" s="110">
+        <v>2</v>
+      </c>
+      <c r="J11" s="110">
         <v>4</v>
       </c>
-      <c r="K11" s="79">
+      <c r="K11" s="111">
         <v>4</v>
       </c>
     </row>
@@ -9123,28 +9123,28 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="72">
+      <c r="D12" s="112">
         <v>18</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="113">
         <v>31</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="113">
         <v>15</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="113">
         <v>6</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="113">
         <v>4</v>
       </c>
-      <c r="I12" s="73">
-        <v>2</v>
-      </c>
-      <c r="J12" s="42">
+      <c r="I12" s="113">
+        <v>2</v>
+      </c>
+      <c r="J12" s="113">
         <v>11</v>
       </c>
-      <c r="K12" s="80">
+      <c r="K12" s="114">
         <v>23</v>
       </c>
     </row>
@@ -9158,28 +9158,28 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="81">
+      <c r="D13" s="115">
         <v>4</v>
       </c>
-      <c r="E13" s="76">
+      <c r="E13" s="116">
         <v>61</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="116">
         <v>9</v>
       </c>
-      <c r="G13" s="77">
+      <c r="G13" s="116">
         <v>11</v>
       </c>
-      <c r="H13" s="76">
+      <c r="H13" s="116">
         <v>32</v>
       </c>
-      <c r="I13" s="76">
+      <c r="I13" s="116">
         <v>11</v>
       </c>
-      <c r="J13" s="77">
+      <c r="J13" s="116">
         <v>9</v>
       </c>
-      <c r="K13" s="82">
+      <c r="K13" s="117">
         <v>10</v>
       </c>
     </row>
@@ -9188,28 +9188,28 @@
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="71">
+      <c r="D14" s="109">
         <v>11</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="110">
         <v>17</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="110">
         <v>47</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="110">
         <v>9</v>
       </c>
-      <c r="H14" s="69">
+      <c r="H14" s="110">
         <v>9</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="110">
         <v>25</v>
       </c>
-      <c r="J14" s="69">
+      <c r="J14" s="110">
         <v>14</v>
       </c>
-      <c r="K14" s="79">
+      <c r="K14" s="111">
         <v>59</v>
       </c>
     </row>
@@ -9221,28 +9221,28 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="68">
-        <v>2</v>
-      </c>
-      <c r="E15" s="19">
-        <v>2</v>
-      </c>
-      <c r="F15" s="19">
-        <v>2</v>
-      </c>
-      <c r="G15" s="19">
-        <v>2</v>
-      </c>
-      <c r="H15" s="69">
-        <v>2</v>
-      </c>
-      <c r="I15" s="69">
-        <v>2</v>
-      </c>
-      <c r="J15" s="19">
-        <v>2</v>
-      </c>
-      <c r="K15" s="70">
+      <c r="D15" s="109">
+        <v>2</v>
+      </c>
+      <c r="E15" s="110">
+        <v>2</v>
+      </c>
+      <c r="F15" s="110">
+        <v>2</v>
+      </c>
+      <c r="G15" s="110">
+        <v>2</v>
+      </c>
+      <c r="H15" s="110">
+        <v>2</v>
+      </c>
+      <c r="I15" s="110">
+        <v>2</v>
+      </c>
+      <c r="J15" s="110">
+        <v>2</v>
+      </c>
+      <c r="K15" s="111">
         <v>2</v>
       </c>
     </row>
@@ -9252,28 +9252,28 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="83">
-        <v>2</v>
-      </c>
-      <c r="E16" s="73">
-        <v>2</v>
-      </c>
-      <c r="F16" s="42">
+      <c r="D16" s="112">
+        <v>2</v>
+      </c>
+      <c r="E16" s="113">
+        <v>2</v>
+      </c>
+      <c r="F16" s="113">
         <v>11</v>
       </c>
-      <c r="G16" s="42">
-        <v>2</v>
-      </c>
-      <c r="H16" s="73">
-        <v>2</v>
-      </c>
-      <c r="I16" s="42">
-        <v>2</v>
-      </c>
-      <c r="J16" s="42">
-        <v>2</v>
-      </c>
-      <c r="K16" s="80">
+      <c r="G16" s="113">
+        <v>2</v>
+      </c>
+      <c r="H16" s="113">
+        <v>2</v>
+      </c>
+      <c r="I16" s="113">
+        <v>2</v>
+      </c>
+      <c r="J16" s="113">
+        <v>2</v>
+      </c>
+      <c r="K16" s="114">
         <v>2</v>
       </c>
     </row>
@@ -9287,28 +9287,28 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="75">
+      <c r="D17" s="115">
         <v>3</v>
       </c>
-      <c r="E17" s="77">
+      <c r="E17" s="116">
         <v>168</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="116">
         <v>10</v>
       </c>
-      <c r="G17" s="76">
+      <c r="G17" s="116">
         <v>101</v>
       </c>
-      <c r="H17" s="76">
+      <c r="H17" s="116">
         <v>134</v>
       </c>
-      <c r="I17" s="77">
+      <c r="I17" s="116">
         <v>41</v>
       </c>
-      <c r="J17" s="77">
+      <c r="J17" s="116">
         <v>11</v>
       </c>
-      <c r="K17" s="82">
+      <c r="K17" s="117">
         <v>150</v>
       </c>
     </row>
@@ -9317,28 +9317,28 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="71">
+      <c r="D18" s="109">
         <v>260</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="110">
         <v>139</v>
       </c>
-      <c r="F18" s="69">
+      <c r="F18" s="110">
         <v>26</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="110">
         <v>106</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="110">
         <v>120</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="110">
         <v>67</v>
       </c>
-      <c r="J18" s="69">
+      <c r="J18" s="110">
         <v>11</v>
       </c>
-      <c r="K18" s="70">
+      <c r="K18" s="111">
         <v>137</v>
       </c>
     </row>
@@ -9350,28 +9350,28 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="71">
+      <c r="D19" s="109">
         <v>4</v>
       </c>
-      <c r="E19" s="69">
+      <c r="E19" s="110">
         <v>8</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="110">
         <v>42</v>
       </c>
-      <c r="G19" s="69">
+      <c r="G19" s="110">
         <v>6</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="110">
         <v>5</v>
       </c>
-      <c r="I19" s="69">
+      <c r="I19" s="110">
         <v>4</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="110">
         <v>8</v>
       </c>
-      <c r="K19" s="70">
+      <c r="K19" s="111">
         <v>14</v>
       </c>
     </row>
@@ -9381,28 +9381,28 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="83">
+      <c r="D20" s="112">
         <v>20</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="113">
         <v>15</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="113">
         <v>16</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="113">
         <v>3</v>
       </c>
-      <c r="H20" s="73">
+      <c r="H20" s="113">
         <v>4</v>
       </c>
-      <c r="I20" s="42">
+      <c r="I20" s="113">
         <v>6</v>
       </c>
-      <c r="J20" s="73">
+      <c r="J20" s="113">
         <v>22</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="114">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished highlighting best acc mean
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80786063-2532-4F57-BDDB-1F05AA39AB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8886214-9FF6-49EA-B0AB-E013CA7A4270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -651,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -992,6 +992,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7113,8 +7128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7773,16 +7788,16 @@
       <c r="E23" s="98">
         <v>0.86943005181347099</v>
       </c>
-      <c r="F23" s="98">
+      <c r="F23" s="114">
         <v>0.89378238341968896</v>
       </c>
       <c r="G23" s="98">
         <v>0.88618307426597598</v>
       </c>
-      <c r="H23" s="98">
+      <c r="H23" s="114">
         <v>0.90449050086355798</v>
       </c>
-      <c r="I23" s="98">
+      <c r="I23" s="114">
         <v>0.92245250431778902</v>
       </c>
       <c r="J23" s="98">
@@ -7797,7 +7812,7 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="100">
+      <c r="D24" s="116">
         <v>0.90587219343696002</v>
       </c>
       <c r="E24" s="101">
@@ -7812,10 +7827,10 @@
       <c r="H24" s="101">
         <v>0.88013816925734001</v>
       </c>
-      <c r="I24" s="101">
+      <c r="I24" s="115">
         <v>0.92867012089809997</v>
       </c>
-      <c r="J24" s="101">
+      <c r="J24" s="115">
         <v>0.90189982728842799</v>
       </c>
       <c r="K24" s="102">
@@ -7830,19 +7845,19 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="97">
+      <c r="D25" s="117">
         <v>0.87512953367875701</v>
       </c>
       <c r="E25" s="98">
         <v>0.86822107081174504</v>
       </c>
-      <c r="F25" s="98">
+      <c r="F25" s="114">
         <v>0.87944732297063899</v>
       </c>
       <c r="G25" s="98">
         <v>0.86234887737478405</v>
       </c>
-      <c r="H25" s="98">
+      <c r="H25" s="114">
         <v>0.87495682210708103</v>
       </c>
       <c r="I25" s="98">
@@ -7860,13 +7875,13 @@
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="100">
+      <c r="D26" s="116">
         <v>0.90172711571675301</v>
       </c>
       <c r="E26" s="101">
         <v>0.86390328151986195</v>
       </c>
-      <c r="F26" s="101">
+      <c r="F26" s="115">
         <v>0.88531951640759898</v>
       </c>
       <c r="G26" s="101">
@@ -7878,7 +7893,7 @@
       <c r="I26" s="101">
         <v>0.83816925734024195</v>
       </c>
-      <c r="J26" s="101">
+      <c r="J26" s="115">
         <v>0.899309153713299</v>
       </c>
       <c r="K26" s="102">
@@ -7893,7 +7908,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="97">
+      <c r="D27" s="117">
         <v>0.87858376511226299</v>
       </c>
       <c r="E27" s="98">
@@ -7902,10 +7917,10 @@
       <c r="F27" s="98">
         <v>0.87150259067357505</v>
       </c>
-      <c r="G27" s="98">
+      <c r="G27" s="114">
         <v>0.88480138169257305</v>
       </c>
-      <c r="H27" s="98">
+      <c r="H27" s="114">
         <v>0.88549222797927496</v>
       </c>
       <c r="I27" s="98">
@@ -7924,13 +7939,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="100">
+      <c r="D28" s="116">
         <v>0.77409326424870495</v>
       </c>
       <c r="E28" s="101">
         <v>0.61139896373057001</v>
       </c>
-      <c r="F28" s="101">
+      <c r="F28" s="115">
         <v>0.79689119170984501</v>
       </c>
       <c r="G28" s="101">
@@ -7939,7 +7954,7 @@
       <c r="H28" s="101">
         <v>0.77443868739205501</v>
       </c>
-      <c r="I28" s="101">
+      <c r="I28" s="115">
         <v>0.791191709844559</v>
       </c>
       <c r="J28" s="101">
@@ -7963,19 +7978,19 @@
       <c r="E29" s="16">
         <v>0.87789291882556098</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="118">
         <v>0.899309153713299</v>
       </c>
       <c r="G29" s="16">
         <v>0.87754749568221102</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="118">
         <v>0.88151986183074305</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="118">
         <v>0.88842832469775501</v>
       </c>
-      <c r="J29" s="16">
+      <c r="J29" s="118">
         <v>0.88290155440414497</v>
       </c>
       <c r="K29" s="104">
@@ -7988,10 +8003,10 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="100">
+      <c r="D30" s="116">
         <v>0.88255613126079402</v>
       </c>
-      <c r="E30" s="101">
+      <c r="E30" s="115">
         <v>0.88013816925734001</v>
       </c>
       <c r="F30" s="101">
@@ -8003,10 +8018,10 @@
       <c r="H30" s="101">
         <v>0.87409326424870504</v>
       </c>
-      <c r="I30" s="101">
+      <c r="I30" s="115">
         <v>0.90241796200345403</v>
       </c>
-      <c r="J30" s="101">
+      <c r="J30" s="115">
         <v>0.91174438687392101</v>
       </c>
       <c r="K30" s="102">

</xml_diff>